<commit_message>
descriptive statistics for corpus2
</commit_message>
<xml_diff>
--- a/Experiment 2b/Corpus/Corpus2.xlsx
+++ b/Experiment 2b/Corpus/Corpus2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R\preview_costs\Experiment 3\Corpus\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R\preview_costs\Experiment 2b\Corpus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF735D01-21AE-4FBF-B044-E0A808E9DA21}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{584C8E1B-7434-42AA-8F5A-EA2E2E58BDB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -6055,9 +6057,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="5">
     <dxf>
@@ -6420,14 +6422,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T148"/>
+  <dimension ref="A1:T151"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D143" sqref="D143"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A124" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K151" sqref="K151"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="7.44140625" style="1" customWidth="1"/>
     <col min="4" max="5" width="8" style="1" customWidth="1"/>
@@ -15444,7 +15446,7 @@
         <v>836</v>
       </c>
       <c r="F130" s="14">
-        <f t="shared" ref="F130:F140" si="38">LEN(C130)</f>
+        <f t="shared" ref="F130:F139" si="38">LEN(C130)</f>
         <v>5</v>
       </c>
       <c r="G130" s="14">
@@ -16434,26 +16436,80 @@
         <v>4.77536231884058</v>
       </c>
       <c r="K147" s="3">
+        <f>AVERAGE(K2:K139)</f>
+        <v>14.166666666666666</v>
+      </c>
+    </row>
+    <row r="148" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="F148" s="1">
+        <f>STDEV(F2:F139)</f>
+        <v>0.61630066534331529</v>
+      </c>
+      <c r="K148" s="3">
+        <f>STDEV(K2:K139)</f>
+        <v>1.7324019582683963</v>
+      </c>
+      <c r="N148" s="1">
+        <f>AVERAGE(N2:N139)</f>
+        <v>5.6521739130434785</v>
+      </c>
+      <c r="T148">
+        <f>AVERAGE(T2:T139)</f>
+        <v>7.4855072463768115</v>
+      </c>
+    </row>
+    <row r="149" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="F149" s="1">
+        <f>MIN(F2:F139)</f>
+        <v>4</v>
+      </c>
+      <c r="K149" s="3">
+        <f>MIN(K2:K139)</f>
+        <v>9</v>
+      </c>
+      <c r="N149" s="1">
+        <f>STDEV(N2:N139)</f>
+        <v>1.2709682148307737</v>
+      </c>
+      <c r="O149" s="1">
+        <f>STDEV(O2:O139)</f>
+        <v>0.61630066534331529</v>
+      </c>
+      <c r="T149">
+        <f>STDEV(T2:T139)</f>
+        <v>2.1452221814945664</v>
+      </c>
+    </row>
+    <row r="150" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="F150" s="1">
+        <f>MAX(F2:F139)</f>
+        <v>6</v>
+      </c>
+      <c r="K150" s="3">
         <f>MAX(K2:K139)</f>
         <v>18</v>
       </c>
-      <c r="N147" s="1">
+      <c r="N150" s="1">
+        <f>MIN(N2:N139)</f>
+        <v>4</v>
+      </c>
+      <c r="T150">
+        <f>MIN(T2:T139)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="151" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="N151" s="1">
         <f>MAX(N2:N139)</f>
         <v>8</v>
       </c>
-      <c r="O147" s="1">
+      <c r="O151" s="1">
         <f>MAX(O2:O139)</f>
         <v>6</v>
       </c>
-    </row>
-    <row r="148" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="N148" s="1">
-        <f>STDEV(N2:N139)</f>
-        <v>1.2709682148307737</v>
-      </c>
-      <c r="O148" s="1">
-        <f>STDEV(O2:O139)</f>
-        <v>0.61630066534331529</v>
+      <c r="T151">
+        <f>MAX(T2:T139)</f>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -16494,7 +16550,7 @@
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.109375" bestFit="1" customWidth="1"/>

</xml_diff>